<commit_message>
Also look for bailleur by their SIRET number
</commit_message>
<xml_diff>
--- a/apilos_settings/tests/resources/listing_bailleur_ok.xlsx
+++ b/apilos_settings/tests/resources/listing_bailleur_ok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/apilos_settings/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2326ACD5-9CE2-364F-BC24-7FA4477EE99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E37D7B-CB9B-EC4A-8352-5087FAF36D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="34980" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,14 +27,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Degré de Motivation'!$A$1:$M$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Informations Participants'!$D$1:$I$28</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="440">
   <si>
     <t>Nom</t>
   </si>
@@ -5466,9 +5469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
@@ -5535,8 +5538,8 @@
       <c r="B3" s="95" t="s">
         <v>435</v>
       </c>
-      <c r="C3" s="98" t="s">
-        <v>439</v>
+      <c r="C3" s="98">
+        <v>987654321</v>
       </c>
       <c r="D3" s="97"/>
       <c r="E3" s="95"/>

</xml_diff>

<commit_message>
Améliorer le traitement du fichier d'utilisateurs bailleur (#428)
* Improve empy line management in XLSX file processing

* Also look for bailleur by their SIRET number
</commit_message>
<xml_diff>
--- a/apilos_settings/tests/resources/listing_bailleur_ok.xlsx
+++ b/apilos_settings/tests/resources/listing_bailleur_ok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitou/Pro/apilos/apilos_settings/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2326ACD5-9CE2-364F-BC24-7FA4477EE99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E37D7B-CB9B-EC4A-8352-5087FAF36D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="34980" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,14 +27,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Degré de Motivation'!$A$1:$M$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Informations Participants'!$D$1:$I$28</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="440">
   <si>
     <t>Nom</t>
   </si>
@@ -5466,9 +5469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
@@ -5535,8 +5538,8 @@
       <c r="B3" s="95" t="s">
         <v>435</v>
       </c>
-      <c r="C3" s="98" t="s">
-        <v>439</v>
+      <c r="C3" s="98">
+        <v>987654321</v>
       </c>
       <c r="D3" s="97"/>
       <c r="E3" s="95"/>

</xml_diff>